<commit_message>
diverse Updates, einige Bilder hinzugefügt
</commit_message>
<xml_diff>
--- a/data/termine.xlsx
+++ b/data/termine.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://corpdir-my.sharepoint.com/personal/mantief_emea_corpdir_net/Documents/00_DATEN/Musik/trachtenkapelle-riezlern.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0375599D-5BC3-4372-9D99-A2BDF734633F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{0375599D-5BC3-4372-9D99-A2BDF734633F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDD8772A-950D-4F81-A5F2-AFA0101535FD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{1DF396E7-779C-4A65-A8D4-F7271FA83EEB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="316">
   <si>
     <t>Orchester</t>
   </si>
@@ -779,9 +779,6 @@
     <t>19.04. 12:00</t>
   </si>
   <si>
-    <t>TK - Erstkommunion</t>
-  </si>
-  <si>
     <t>0k0ia7333okpi753lo5uf4qts8@google.com</t>
   </si>
   <si>
@@ -815,9 +812,6 @@
     <t>25.04. 22:00</t>
   </si>
   <si>
-    <t>TK - Jahreskonzert</t>
-  </si>
-  <si>
     <t>1pdrmpt3k4b14nh4q4b6r9qngc@google.com</t>
   </si>
   <si>
@@ -830,9 +824,6 @@
     <t>14.06. 12:00</t>
   </si>
   <si>
-    <t>TK - Firmung</t>
-  </si>
-  <si>
     <t>tp08rcuhrkveoglbqu7f47385c@google.com</t>
   </si>
   <si>
@@ -848,9 +839,6 @@
     <t>Gemeindeplatz oder Kurpark</t>
   </si>
   <si>
-    <t>TK - 210 Jahre TK Riezlern</t>
-  </si>
-  <si>
     <t>99e4sqi92sb3jh620iaui5gkr0@google.com</t>
   </si>
   <si>
@@ -866,9 +854,6 @@
     <t>Gemeindeplatz</t>
   </si>
   <si>
-    <t>TK - Sommerkonzert</t>
-  </si>
-  <si>
     <t>aajjt4aq6ndhpp49jltv8sf5t0@google.com</t>
   </si>
   <si>
@@ -899,9 +884,6 @@
     <t>15.08. 18:00</t>
   </si>
   <si>
-    <t>TK - Tag der Blasmusik</t>
-  </si>
-  <si>
     <t>0s38tlv04aiaqp26k5dr7adv1c@google.com</t>
   </si>
   <si>
@@ -926,9 +908,6 @@
     <t>Oberstdorf</t>
   </si>
   <si>
-    <t>TK - Musikfest Oberstdorf</t>
-  </si>
-  <si>
     <t>vrfm6bccp7lki6478f6jtft72c@google.com</t>
   </si>
   <si>
@@ -968,9 +947,6 @@
     <t>18.10. 12:00</t>
   </si>
   <si>
-    <t>TK - Kriegergedenken</t>
-  </si>
-  <si>
     <t>rc7l5e5t64klnd4fjohvhk7uc4@google.com</t>
   </si>
   <si>
@@ -1005,6 +981,9 @@
   </si>
   <si>
     <t>frei</t>
+  </si>
+  <si>
+    <t>TK Riezlern @ Musikfest Oberstdorf</t>
   </si>
 </sst>
 </file>
@@ -1652,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B97407-46BC-4778-A645-CBC9276C5DF5}">
   <dimension ref="A1:T78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="O65" sqref="O65:O77"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="S76" sqref="S76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,16 +1675,16 @@
         <v>11</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -3214,7 +3193,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>12</v>
       </c>
@@ -3246,7 +3225,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>12</v>
       </c>
@@ -3278,7 +3257,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
         <v>12</v>
       </c>
@@ -3310,7 +3289,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>12</v>
       </c>
@@ -3342,7 +3321,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
         <v>12</v>
       </c>
@@ -3374,7 +3353,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>12</v>
       </c>
@@ -3406,7 +3385,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
         <v>12</v>
       </c>
@@ -3438,7 +3417,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>12</v>
       </c>
@@ -3470,7 +3449,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="12" t="s">
         <v>12</v>
       </c>
@@ -3502,7 +3481,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>12</v>
       </c>
@@ -3534,7 +3513,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
         <v>12</v>
       </c>
@@ -3566,7 +3545,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>12</v>
       </c>
@@ -3598,7 +3577,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="12" t="s">
         <v>12</v>
       </c>
@@ -3630,7 +3609,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>12</v>
       </c>
@@ -3651,7 +3630,7 @@
         <v>116</v>
       </c>
       <c r="H62" s="9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="I62" s="7"/>
       <c r="J62" s="10">
@@ -3659,10 +3638,22 @@
       </c>
       <c r="K62" s="7"/>
       <c r="L62" s="19" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+      <c r="M62" t="s">
+        <v>308</v>
+      </c>
+      <c r="N62" t="s">
+        <v>313</v>
+      </c>
+      <c r="O62" t="s">
+        <v>314</v>
+      </c>
+      <c r="P62" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="12" t="s">
         <v>12</v>
       </c>
@@ -3670,14 +3661,14 @@
         <v>13</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D63" s="14"/>
       <c r="E63" s="15">
         <v>2</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G63" s="16" t="s">
         <v>16</v>
@@ -3691,10 +3682,10 @@
       </c>
       <c r="K63" s="14"/>
       <c r="L63" s="18" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>12</v>
       </c>
@@ -3702,17 +3693,17 @@
         <v>113</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="8">
         <v>2</v>
       </c>
       <c r="F64" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="G64" s="9" t="s">
         <v>253</v>
-      </c>
-      <c r="G64" s="9" t="s">
-        <v>254</v>
       </c>
       <c r="H64" s="9" t="s">
         <v>117</v>
@@ -3723,7 +3714,7 @@
       </c>
       <c r="K64" s="7"/>
       <c r="L64" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3731,23 +3722,23 @@
         <v>12</v>
       </c>
       <c r="B65" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="C65" s="13" t="s">
         <v>256</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>257</v>
       </c>
       <c r="D65" s="14"/>
       <c r="E65" s="15">
         <v>2</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H65" s="16" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I65" s="14"/>
       <c r="J65" s="17">
@@ -3755,19 +3746,19 @@
       </c>
       <c r="K65" s="14"/>
       <c r="L65" s="18" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M65" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N65" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O65" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="P65" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3775,23 +3766,23 @@
         <v>12</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="8">
         <v>2</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G66" s="9" t="s">
         <v>116</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I66" s="7"/>
       <c r="J66" s="10">
@@ -3799,19 +3790,19 @@
       </c>
       <c r="K66" s="7"/>
       <c r="L66" s="19" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="M66" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N66" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O66" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="P66" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3819,23 +3810,23 @@
         <v>12</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D67" s="14"/>
       <c r="E67" s="15">
         <v>6</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G67" s="16" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="I67" s="14"/>
       <c r="J67" s="17">
@@ -3843,19 +3834,19 @@
       </c>
       <c r="K67" s="14"/>
       <c r="L67" s="18" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="M67" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N67" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O67" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="P67" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="68" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3863,23 +3854,23 @@
         <v>12</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="8">
         <v>1</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="I68" s="7"/>
       <c r="J68" s="10">
@@ -3887,19 +3878,19 @@
       </c>
       <c r="K68" s="7"/>
       <c r="L68" s="19" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="M68" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N68" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O68" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="P68" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="69" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3907,23 +3898,23 @@
         <v>12</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D69" s="14"/>
       <c r="E69" s="15">
         <v>1</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="G69" s="16" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H69" s="16" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="I69" s="14"/>
       <c r="J69" s="17">
@@ -3931,19 +3922,19 @@
       </c>
       <c r="K69" s="14"/>
       <c r="L69" s="18" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="M69" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N69" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O69" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="P69" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3951,23 +3942,23 @@
         <v>12</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D70" s="7"/>
       <c r="E70" s="8">
         <v>1</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="I70" s="7"/>
       <c r="J70" s="10">
@@ -3975,19 +3966,19 @@
       </c>
       <c r="K70" s="7"/>
       <c r="L70" s="19" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="M70" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N70" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O70" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="P70" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="71" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3995,21 +3986,21 @@
         <v>12</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D71" s="14"/>
       <c r="E71" s="15">
         <v>11</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="G71" s="14"/>
       <c r="H71" s="16" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="I71" s="14"/>
       <c r="J71" s="17">
@@ -4017,19 +4008,19 @@
       </c>
       <c r="K71" s="14"/>
       <c r="L71" s="18" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="M71" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N71" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O71" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="P71" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4037,23 +4028,23 @@
         <v>12</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="8">
         <v>1</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H72" s="9" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="I72" s="7"/>
       <c r="J72" s="10">
@@ -4061,19 +4052,19 @@
       </c>
       <c r="K72" s="7"/>
       <c r="L72" s="19" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="M72" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N72" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O72" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="P72" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="73" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4081,23 +4072,23 @@
         <v>12</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D73" s="14"/>
       <c r="E73" s="15">
         <v>6</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="G73" s="16" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="H73" s="16" t="s">
-        <v>296</v>
+        <v>315</v>
       </c>
       <c r="I73" s="14"/>
       <c r="J73" s="17">
@@ -4105,19 +4096,19 @@
       </c>
       <c r="K73" s="14"/>
       <c r="L73" s="18" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="M73" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N73" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O73" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="P73" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="74" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4125,23 +4116,23 @@
         <v>12</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="8">
         <v>1</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="I74" s="7"/>
       <c r="J74" s="10">
@@ -4149,19 +4140,19 @@
       </c>
       <c r="K74" s="7"/>
       <c r="L74" s="19" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="M74" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N74" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O74" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="P74" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="75" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4169,23 +4160,23 @@
         <v>12</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D75" s="14"/>
       <c r="E75" s="15">
         <v>1</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="G75" s="16" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H75" s="16" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="I75" s="14"/>
       <c r="J75" s="17">
@@ -4193,19 +4184,19 @@
       </c>
       <c r="K75" s="14"/>
       <c r="L75" s="18" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="M75" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N75" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O75" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="P75" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="76" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4213,23 +4204,23 @@
         <v>12</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="8">
         <v>1</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H76" s="9" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="I76" s="7"/>
       <c r="J76" s="10">
@@ -4237,19 +4228,19 @@
       </c>
       <c r="K76" s="7"/>
       <c r="L76" s="19" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="M76" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N76" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O76" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="P76" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="77" spans="1:16" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4257,23 +4248,23 @@
         <v>12</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="D77" s="14"/>
       <c r="E77" s="15">
         <v>2</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="G77" s="16" t="s">
         <v>116</v>
       </c>
       <c r="H77" s="16" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="I77" s="14"/>
       <c r="J77" s="17">
@@ -4281,19 +4272,19 @@
       </c>
       <c r="K77" s="14"/>
       <c r="L77" s="18" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="M77" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="N77" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="O77" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="P77" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="78" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update erkennung der Terminart
</commit_message>
<xml_diff>
--- a/data/termine.xlsx
+++ b/data/termine.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="16" documentId="8_{0375599D-5BC3-4372-9D99-A2BDF734633F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDD8772A-950D-4F81-A5F2-AFA0101535FD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{1DF396E7-779C-4A65-A8D4-F7271FA83EEB}"/>
+    <workbookView minimized="1" xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12645" xr2:uid="{1DF396E7-779C-4A65-A8D4-F7271FA83EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1632,7 +1632,7 @@
   <dimension ref="A1:T78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="S76" sqref="S76"/>
+      <selection activeCell="R75" sqref="R75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>